<commit_message>
VAN-1761: Prepare test cases and write test scripts for smoke testing
</commit_message>
<xml_diff>
--- a/ui-testsuite/src/main/resources/TestData/Unassigned_ATR.xlsx
+++ b/ui-testsuite/src/main/resources/TestData/Unassigned_ATR.xlsx
@@ -630,9 +630,6 @@
     <t>SINERGIT SA -  DO</t>
   </si>
   <si>
-    <t>08138265</t>
-  </si>
-  <si>
     <t>LAC - MUNOZ, HECTOR GERARDO</t>
   </si>
   <si>
@@ -669,7 +666,10 @@
     <t>Q3</t>
   </si>
   <si>
-    <t>2152430001</t>
+    <t>abcd</t>
+  </si>
+  <si>
+    <t>215243fdgb699</t>
   </si>
 </sst>
 </file>
@@ -1111,8 +1111,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FF2"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="BU1" workbookViewId="0">
-      <selection activeCell="CD2" sqref="CD2"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1910,7 +1910,7 @@
         <v>1</v>
       </c>
       <c r="BW2" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="BX2" s="1" t="s">
         <v>197</v>
@@ -1919,7 +1919,7 @@
         <v>198</v>
       </c>
       <c r="BZ2" s="22" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="CA2" s="1" t="s">
         <v>199</v>
@@ -1930,26 +1930,26 @@
       <c r="CC2" s="1" t="s">
         <v>201</v>
       </c>
-      <c r="CE2" s="1" t="s">
+      <c r="CD2" s="1" t="s">
+        <v>214</v>
+      </c>
+      <c r="CF2" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="CF2" s="1" t="s">
-        <v>203</v>
-      </c>
       <c r="CG2" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CH2" s="1" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="CJ2" s="1" t="s">
         <v>173</v>
       </c>
       <c r="CK2" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="CL2" s="1" t="s">
         <v>204</v>
-      </c>
-      <c r="CL2" s="1" t="s">
-        <v>205</v>
       </c>
       <c r="CP2" s="3">
         <v>1</v>
@@ -1973,16 +1973,16 @@
         <v>3975.6923076923076</v>
       </c>
       <c r="CW2" s="1" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="CZ2" s="1" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="DA2" s="2" t="s">
         <v>182</v>
       </c>
       <c r="DC2" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="DF2" s="2" t="s">
         <v>196</v>
@@ -1991,31 +1991,31 @@
         <v>187</v>
       </c>
       <c r="DL2" s="1" t="s">
+        <v>206</v>
+      </c>
+      <c r="DM2" s="22" t="s">
+        <v>209</v>
+      </c>
+      <c r="DN2" s="23" t="s">
+        <v>210</v>
+      </c>
+      <c r="DO2" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="DM2" s="22" t="s">
-        <v>210</v>
-      </c>
-      <c r="DN2" s="23" t="s">
-        <v>211</v>
-      </c>
-      <c r="DO2" s="1" t="s">
+      <c r="DP2" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="DP2" s="1" t="s">
-        <v>209</v>
-      </c>
       <c r="DQ2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="DR2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="DS2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="DU2" s="1" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
   </sheetData>

</xml_diff>